<commit_message>
drugi problem drugega dne
</commit_message>
<xml_diff>
--- a/2021/02/2021_02_1.xlsx
+++ b/2021/02/2021_02_1.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18468" windowHeight="9335"/>
+    <workbookView windowWidth="18468" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="problem 1" sheetId="1" r:id="rId1"/>
+    <sheet name="problem 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'problem 1'!$A$1:$A$1001</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -37,8 +38,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -50,36 +51,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -103,6 +74,37 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -111,7 +113,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,22 +167,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,45 +194,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -203,7 +204,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,169 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,17 +398,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -429,9 +433,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,44 +489,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -517,130 +518,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -972,7 +973,7 @@
   <sheetPr/>
   <dimension ref="A2:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A377" workbookViewId="0">
+    <sheetView topLeftCell="A377" workbookViewId="0">
       <selection activeCell="H400" sqref="H400"/>
     </sheetView>
   </sheetViews>
@@ -15013,4 +15014,20 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>